<commit_message>
Modificación de la bitácora
</commit_message>
<xml_diff>
--- a/Bitácora-Steven.xlsx
+++ b/Bitácora-Steven.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\Desktop\Proyecto 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\Documents\Repositorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,9 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Se creó el archivo html de la aplicación web administradora, y se implemento la interfaz de gestión de roles. Además se añadió  bootstrap a la página, se creó el menu despleglable y los logos de la aplicación.</t>
+  </si>
+  <si>
+    <t>Se realizó la interfaz de gestión de clientes, se creó el repositorio en github y se creó el primer commit.</t>
   </si>
 </sst>
 </file>
@@ -401,7 +404,7 @@
   <dimension ref="A2:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,11 +430,19 @@
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>42863.416666666664</v>
+      </c>
+      <c r="C3" s="2">
+        <v>42862.541666666664</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>

</xml_diff>

<commit_message>
Actualización de la bitácora.
</commit_message>
<xml_diff>
--- a/Bitácora-Steven.xlsx
+++ b/Bitácora-Steven.xlsx
@@ -24,12 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Se creó el archivo html de la aplicación web administradora, y se implemento la interfaz de gestión de roles. Además se añadió  bootstrap a la página, se creó el menu despleglable y los logos de la aplicación.</t>
   </si>
   <si>
     <t>Se realizó la interfaz de gestión de clientes, se creó el repositorio en github y se creó el primer commit.</t>
+  </si>
+  <si>
+    <t>Se realizó un cambio en la interfaz de clientes y se creó la interfaz de gestión de cuentas.</t>
   </si>
 </sst>
 </file>
@@ -404,7 +407,7 @@
   <dimension ref="A2:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,11 +447,19 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>42864.916666666664</v>
+      </c>
+      <c r="C4" s="2">
+        <v>42865.104166666664</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.1875</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>

</xml_diff>

<commit_message>
Creacion de pestaña empleados y login, se crea la carpeta de la web cliente.
</commit_message>
<xml_diff>
--- a/Bitácora-Steven.xlsx
+++ b/Bitácora-Steven.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Se creó el archivo html de la aplicación web administradora, y se implemento la interfaz de gestión de roles. Además se añadió  bootstrap a la página, se creó el menu despleglable y los logos de la aplicación.</t>
   </si>
@@ -33,6 +33,12 @@
   </si>
   <si>
     <t>Se realizó un cambio en la interfaz de clientes y se creó la interfaz de gestión de cuentas.</t>
+  </si>
+  <si>
+    <t>Se crearon el resto de pestañas de la web administradora.</t>
+  </si>
+  <si>
+    <t>Se añadio la pestaña de empleados a la web administradora y se creó el formulario de login.</t>
   </si>
 </sst>
 </file>
@@ -407,7 +413,7 @@
   <dimension ref="A2:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,16 +468,32 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>42870.791666666664</v>
+      </c>
+      <c r="C5" s="2">
+        <v>42870.958333333336</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>42871.833333333336</v>
+      </c>
+      <c r="C6" s="2">
+        <v>42871.958333333336</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>

</xml_diff>

<commit_message>
Finalización de los request de la web administradora.
</commit_message>
<xml_diff>
--- a/Bitácora-Steven.xlsx
+++ b/Bitácora-Steven.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Se creó el archivo html de la aplicación web administradora, y se implemento la interfaz de gestión de roles. Además se añadió  bootstrap a la página, se creó el menu despleglable y los logos de la aplicación.</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>Se crearon los request de Roles, Clientes, Empleados, Cuentas, Tarjetas, Asesores y parte de Préstamos.</t>
+  </si>
+  <si>
+    <t>Finalización de los request de la web administradora.</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
   <dimension ref="A2:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,10 +516,18 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>42878.625</v>
+      </c>
+      <c r="C8" s="2">
+        <v>42879.041666666664</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.41666666666666669</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>

</xml_diff>

<commit_message>
Avance de los request de la web cliente.
</commit_message>
<xml_diff>
--- a/Bitácora-Steven.xlsx
+++ b/Bitácora-Steven.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Se creó el archivo html de la aplicación web administradora, y se implemento la interfaz de gestión de roles. Además se añadió  bootstrap a la página, se creó el menu despleglable y los logos de la aplicación.</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Finalización de los request de la web administradora.</t>
+  </si>
+  <si>
+    <t>Avance de los reques de la web cliente.</t>
   </si>
 </sst>
 </file>
@@ -419,7 +422,7 @@
   <dimension ref="A2:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,10 +533,18 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>42879.041666666664</v>
+      </c>
+      <c r="C9" s="2">
+        <v>42879.125</v>
+      </c>
+      <c r="D9" s="3">
+        <v>8.3333333333333329E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>

</xml_diff>

<commit_message>
FInalización de los request de la web cliente.
</commit_message>
<xml_diff>
--- a/Bitácora-Steven.xlsx
+++ b/Bitácora-Steven.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Se creó el archivo html de la aplicación web administradora, y se implemento la interfaz de gestión de roles. Además se añadió  bootstrap a la página, se creó el menu despleglable y los logos de la aplicación.</t>
   </si>
@@ -47,7 +47,10 @@
     <t>Finalización de los request de la web administradora.</t>
   </si>
   <si>
-    <t>Avance de los reques de la web cliente.</t>
+    <t>Avance de los request de la web cliente.</t>
+  </si>
+  <si>
+    <t>FInalización de los request de la web cliente.</t>
   </si>
 </sst>
 </file>
@@ -421,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,10 +550,18 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>42879.833333333336</v>
+      </c>
+      <c r="C10" s="2">
+        <v>42880.166666666664</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.33333333333333331</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>

</xml_diff>